<commit_message>
Added logic for execution status logging in external text file
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
+++ b/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="96">
   <si>
     <t>Choose Test (Smoke/Regression/Custom/Negative)</t>
   </si>
@@ -392,6 +392,9 @@
   </si>
   <si>
     <t>TCs-016,TCs-017,TCs-018,TCs-019,TCs-020</t>
+  </si>
+  <si>
+    <t>NaN %</t>
   </si>
 </sst>
 </file>
@@ -496,7 +499,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,6 +563,11 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -727,7 +735,7 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="7" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="204">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -867,6 +875,70 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
@@ -1344,7 +1416,7 @@
       <c r="E2" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F2" t="s" s="138">
+      <c r="F2" t="s" s="185">
         <v>83</v>
       </c>
     </row>
@@ -1364,7 +1436,7 @@
       <c r="E3" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F3" t="s" s="123">
+      <c r="F3" t="s" s="191">
         <v>83</v>
       </c>
     </row>
@@ -1384,7 +1456,7 @@
       <c r="E4" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F4" t="s" s="129">
+      <c r="F4" t="s" s="197">
         <v>83</v>
       </c>
     </row>
@@ -1404,7 +1476,7 @@
       <c r="E5" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F5" t="s" s="126">
+      <c r="F5" t="s" s="194">
         <v>83</v>
       </c>
     </row>
@@ -1424,7 +1496,7 @@
       <c r="E6" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F6" t="s" s="132">
+      <c r="F6" t="s" s="200">
         <v>83</v>
       </c>
     </row>
@@ -1444,7 +1516,7 @@
       <c r="E7" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F7" t="s" s="135">
+      <c r="F7" t="s" s="203">
         <v>83</v>
       </c>
     </row>
@@ -1535,7 +1607,7 @@
       <c r="G2" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="139" t="s">
+      <c r="H2" s="183" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1561,7 +1633,7 @@
       <c r="G3" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="H3" s="137" t="s">
+      <c r="H3" s="184" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1638,7 +1710,7 @@
       <c r="F2" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="118" t="s">
+      <c r="G2" s="186" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1661,7 +1733,7 @@
       <c r="F3" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="119" t="s">
+      <c r="G3" s="187" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1680,7 +1752,7 @@
       <c r="F4" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="120" t="s">
+      <c r="G4" s="188" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1701,7 +1773,7 @@
       <c r="F5" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G5" s="121" t="s">
+      <c r="G5" s="189" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1722,7 +1794,7 @@
       <c r="F6" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="122" t="s">
+      <c r="G6" s="190" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1818,7 +1890,7 @@
       <c r="I2" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="J2" s="124" t="s">
+      <c r="J2" s="192" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1850,7 +1922,7 @@
       <c r="I3" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="J3" s="125" t="s">
+      <c r="J3" s="193" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1925,7 +1997,7 @@
       <c r="F2" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="127" t="s">
+      <c r="G2" s="195" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1948,7 +2020,7 @@
       <c r="F3" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="128" t="s">
+      <c r="G3" s="196" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2017,7 +2089,7 @@
       <c r="E2" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="130" t="s">
+      <c r="F2" s="198" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2037,7 +2109,7 @@
       <c r="E3" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="131" t="s">
+      <c r="F3" s="199" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2119,7 +2191,7 @@
       <c r="G2" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="133" t="s">
+      <c r="H2" s="201" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2145,7 +2217,7 @@
       <c r="G3" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="134" t="s">
+      <c r="H3" s="202" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>